<commit_message>
Updated for EA 23.188 Stable. Added Config menu options: Land Expansion, Zone Investment, Temporary Merchant Recruitment, and Experimental Manage Land Traits.
EA 23.188 Stable に対応しました。Config メニューに機能を追加：土地拡張、ゾーン投資、臨時商人の雇用、そして【実験的】土地の特徴の管理。

现已更新至 EA 23.188 Stable。已在 Config 菜单新增功能：土地扩张、区域投资、临时商人招募，以及【实验性】管理土地特性。
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -301,6 +301,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">テント内の最大電力（</t>
     </r>
@@ -318,6 +319,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）を有効または無効にします。</t>
     </r>
@@ -328,6 +330,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">启用或禁用帐篷内的最大电力（</t>
     </r>
@@ -345,9 +348,106 @@
         <sz val="10"/>
         <rFont val="Noto Sans SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）。</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">title03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Land Expansion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">土地拡張</t>
+  </si>
+  <si>
+    <t xml:space="preserve">土地扩张</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tooltip08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expand the tent land.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">テントの敷地面積を拡張します。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">扩张帐篷土地面积。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone Investment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ゾーン投資</t>
+  </si>
+  <si>
+    <t xml:space="preserve">区域投资</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tooltip09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invest to raise this zone’s development and influence. Higher development improves shop inventory quality and variety.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">投資するとゾーンの開発度と影響力が上昇し、開発度が高いほど商店の品揃え（品質と種類）が向上します。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">投资可提升该区域的开发度与影响力；开发度越高，商店的商品品质与种类都会提升。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temporary Merchant Recruitment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">臨時商人の雇用</t>
+  </si>
+  <si>
+    <t xml:space="preserve">临时商人招募</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tooltip10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recruit a temporary merchant. Inventory quality and variety scale with zone development.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">一定期間、商人を雇用します。商店の品揃え（品質と種類）はゾーン開発度に連動します。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">雇佣临时商人。商品的品质与种类随区域开发度提升而提升。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manage Land Traits (Experimental)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">土地の特徴の管理（実験的）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">管理土地特性（实验性）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tooltip11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change this tent’s land traits.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">このテントの土地の特徴を変更します。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">修改此帐篷的土地特性。</t>
   </si>
 </sst>
 </file>
@@ -357,7 +457,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -390,11 +490,6 @@
       <name val="Noto Sans SC"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Noto Sans SC"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -439,7 +534,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -457,10 +552,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -587,13 +678,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="65.95"/>
@@ -847,10 +938,10 @@
       <c r="B18" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>71</v>
       </c>
     </row>
@@ -861,11 +952,123 @@
       <c r="B19" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated for EA 23.200 Stable. Added support for Teleporter usage inside tents.
EA 23.200 Stable に対応しました。テント内でテレポーターの使用を可能にしました。

现已更新至 EA 23.200 Stable。允许在帐篷内使用传送装置。
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -448,6 +448,54 @@
   </si>
   <si>
     <t xml:space="preserve">修改此帐篷的土地特性。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable Teleporter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">テレポーターを有効化</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启用传送装置</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tooltip12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable or disable the use of teleporters inside tents.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">テント内で「テレポーター」を使用できるかを有効または無効にします。</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">启用或禁用帐篷内使用传送装置（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Teleporter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">）。</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -457,7 +505,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -490,6 +538,11 @@
       <name val="Noto Sans SC"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Noto Sans SC"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -534,7 +587,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -552,6 +605,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -678,10 +735,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1071,6 +1128,34 @@
         <v>107</v>
       </c>
     </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Updated for EA 23.209 Stable. Merchants recruited in tents are no longer temporary. They will now persist and automatically revive in the tent where they were hired.
Special thanks to @grueshanker for the ideas and code contributions.

EA 23.209 Stable に対応しました。
テントで雇用した商人は臨時ではなくなりました。雇用されたテントで自動的に復活するようになりました。

现已更新至 EA 23.209 Stable。
在帐篷中雇佣的商人不再是临时的。他们现在会保留，并会在雇佣的帐篷中自动复活。
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -405,13 +405,13 @@
     <t xml:space="preserve">title05</t>
   </si>
   <si>
-    <t xml:space="preserve">Temporary Merchant Recruitment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">臨時商人の雇用</t>
-  </si>
-  <si>
-    <t xml:space="preserve">临时商人招募</t>
+    <t xml:space="preserve">Merchant Recruitment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">商人の雇用</t>
+  </si>
+  <si>
+    <t xml:space="preserve">商人招募</t>
   </si>
   <si>
     <t xml:space="preserve">tooltip10</t>
@@ -476,6 +476,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">启用或禁用帐篷内使用传送装置（</t>
     </r>
@@ -493,6 +494,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）。</t>
     </r>
@@ -505,7 +507,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -538,11 +540,6 @@
       <name val="Noto Sans SC"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Noto Sans SC"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -587,7 +584,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -605,10 +602,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -738,7 +731,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1135,10 +1128,10 @@
       <c r="B28" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1149,10 +1142,10 @@
       <c r="B29" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>115</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new Config option: Enable Dining Spot Sign. Allows dining spot sign effects to work inside tents.
新しい Config オプションを追加しました：食堂の立て札を有効化。テント内で食堂の立て札の効果を有効にできます。

新增 Config 选项：启用食堂招牌。允许帐篷内生效食堂招牌效果。
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -498,6 +498,30 @@
       </rPr>
       <t xml:space="preserve">）。</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable Dining Spot Sign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">食堂の立て札を有効化</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启用食堂招牌</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tooltip13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable or disable dining spot sign effects inside tents.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">テント内で食堂の立て札の効果を有効または無効にします。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启用或禁用帐篷内的食堂招牌效果。</t>
   </si>
 </sst>
 </file>
@@ -507,7 +531,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -540,6 +564,11 @@
       <name val="Noto Sans SC"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Noto Sans SC"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -584,7 +613,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -602,6 +631,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -728,10 +761,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+      <selection pane="topLeft" activeCell="C42" activeCellId="0" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1079,7 +1112,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>96</v>
       </c>
@@ -1147,6 +1180,34 @@
       </c>
       <c r="D29" s="4" t="s">
         <v>115</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>